<commit_message>
deleted supply in disjuncts
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input.xlsx
+++ b/src/pv_optimizer_contracting/data_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F19EBF-B21A-4EE5-A0B9-B5718065C1FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E63067-A0DD-4526-9BD7-62D7553BDCB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -584,7 +584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9740660E-AB78-4CFF-914A-8631BC8F2D6A}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -647,7 +647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33AEF11-6D95-4C68-8F05-ED28777DD177}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added max capacity for all options
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input.xlsx
+++ b/src/pv_optimizer_contracting/data_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66229C6B-037E-4EBC-B171-72EE7CCD98DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298AA5D7-4158-4BA8-9F0B-B8AB21541CFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>PV</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>c_var [€/kWh]</t>
+  </si>
+  <si>
+    <t>Capacity limit grid</t>
   </si>
 </sst>
 </file>
@@ -459,13 +462,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -519,10 +523,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -530,9 +534,10 @@
     <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -545,8 +550,11 @@
       <c r="D1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -559,8 +567,11 @@
       <c r="D2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.08</v>
       </c>
@@ -572,6 +583,9 @@
       </c>
       <c r="D3">
         <v>1</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -583,7 +597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33AEF11-6D95-4C68-8F05-ED28777DD177}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -702,10 +716,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
added constraint demand in every timestep
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input.xlsx
+++ b/src/pv_optimizer_contracting/data_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298AA5D7-4158-4BA8-9F0B-B8AB21541CFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E29FD1-C64A-44FD-B1AC-714FA0E7EEB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -459,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F6BA0A-853F-4A52-83CB-1D40EBCA633B}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -512,8 +512,116 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -525,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -576,7 +684,7 @@
         <v>0.08</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -598,7 +706,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -670,10 +778,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF5F245-D841-4F1D-BA61-85398CE8385D}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -694,7 +802,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -703,7 +811,183 @@
         <v>2</v>
       </c>
       <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
         <v>20</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -713,10 +997,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95034383-FE85-4F68-924D-0BEBCE2AD864}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -741,10 +1025,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2E-3</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>2E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -752,10 +1036,258 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2E-3</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>2E-3</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1.4E-2</v>
+      </c>
+      <c r="C10">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C12">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1E-3</v>
+      </c>
+      <c r="C14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C15">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C26">
+        <f>SUM(C2:C25)</f>
+        <v>3.9E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added charging time constraint
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input.xlsx
+++ b/src/pv_optimizer_contracting/data_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC12722-F954-44E2-A087-D1C2FBFF31B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220B0C85-4734-4EA9-A71B-B30E80DE7D4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -18,8 +18,6 @@
     <sheet name="Cost" sheetId="1" r:id="rId3"/>
     <sheet name="Demand" sheetId="11" r:id="rId4"/>
     <sheet name="irradiation" sheetId="12" r:id="rId5"/>
-    <sheet name="test" sheetId="13" r:id="rId6"/>
-    <sheet name="test_date" sheetId="14" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>PV</t>
   </si>
@@ -641,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1008,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95034383-FE85-4F68-924D-0BEBCE2AD864}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1303,291 +1301,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C96F09-3BD7-4D81-B4D1-D83559F5209A}">
-  <dimension ref="A1:A25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.90625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="3">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="3">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="3">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="3">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCCF2BE2-4255-4C8D-A430-33CC06251F7A}">
-  <dimension ref="A1:A25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.90625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>44197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
-        <v>44197.041666666664</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
-        <v>44197.083333333299</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
-        <v>44197.125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
-        <v>44197.166666666701</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
-        <v>44197.208333333299</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
-        <v>44197.25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
-        <v>44197.291666666701</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
-        <v>44197.333333333299</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
-        <v>44197.375</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
-        <v>44197.416666666701</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
-        <v>44197.458333333299</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
-        <v>44197.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
-        <v>44197.541666666701</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
-        <v>44197.583333333299</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
-        <v>44197.625</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
-        <v>44197.666666666701</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
-        <v>44197.708333333299</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
-        <v>44197.75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
-        <v>44197.791666666701</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
-        <v>44197.833333333299</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2">
-        <v>44197.875</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2">
-        <v>44197.916666666701</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
-        <v>44197.958333333299</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
created output file, hard coded inputs
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input.xlsx
+++ b/src/pv_optimizer_contracting/data_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220B0C85-4734-4EA9-A71B-B30E80DE7D4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC0C7ED-F70D-4B3A-A6A0-268607BF70A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -114,7 +114,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -148,7 +148,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -467,7 +467,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -690,7 +690,7 @@
         <v>0.08</v>
       </c>
       <c r="B3">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -786,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF5F245-D841-4F1D-BA61-85398CE8385D}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1004,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95034383-FE85-4F68-924D-0BEBCE2AD864}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1292,12 +1292,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C26">
-        <f>SUM(C2:C25)</f>
-        <v>3.9E-2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added simple visualisation of model results (24h)
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input.xlsx
+++ b/src/pv_optimizer_contracting/data_input.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC0C7ED-F70D-4B3A-A6A0-268607BF70A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723FA865-1564-4217-84EA-6E3E075477E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
     <sheet name="General Data" sheetId="5" r:id="rId2"/>
     <sheet name="Cost" sheetId="1" r:id="rId3"/>
-    <sheet name="Demand" sheetId="11" r:id="rId4"/>
-    <sheet name="irradiation" sheetId="12" r:id="rId5"/>
+    <sheet name="Demand" sheetId="13" r:id="rId4"/>
+    <sheet name="irradiation" sheetId="15" r:id="rId5"/>
+    <sheet name="irradiation_winter" sheetId="12" r:id="rId6"/>
+    <sheet name="Tabelle1" sheetId="14" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>PV</t>
   </si>
@@ -145,9 +147,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -466,20 +467,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F6BA0A-853F-4A52-83CB-1D40EBCA633B}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="3"/>
+    <col min="1" max="1" width="25.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
@@ -494,7 +495,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>44197</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -508,7 +509,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>44197.041666666664</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -519,7 +520,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>44197.083333333299</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -527,107 +528,107 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>44197.125</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
-        <v>44197.166666666701</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>44197.208333333299</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>44197.25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
-        <v>44197.291666666701</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>44197.333333333299</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>44197.375</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
-        <v>44197.416666666701</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
-        <v>44197.458333333299</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
-        <v>44197.5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
-        <v>44197.541666666701</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
-        <v>44197.583333333299</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
-        <v>44197.625</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
-        <v>44197.666666666701</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
-        <v>44197.708333333299</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
-        <v>44197.75</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
-        <v>44197.791666666701</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
-        <v>44197.833333333299</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
-        <v>44197.875</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
-        <v>44197.916666666701</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
-        <v>44197.958333333299</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -639,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -690,7 +691,7 @@
         <v>0.08</v>
       </c>
       <c r="B3">
-        <v>20000</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -783,143 +784,141 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF5F245-D841-4F1D-BA61-85398CE8385D}">
-  <dimension ref="A1:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CDCAAEF-9BC9-4D67-B5C1-5585BDAAB9DD}">
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="3"/>
-    <col min="5" max="5" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>44197</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>44197.041666666664</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>44197.083333333299</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>44197.125</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
-        <v>44197.166666666701</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>44197.208333333299</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>44197.25</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
-        <v>44197.291666666701</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>44197.333333333299</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>44197.375</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
-        <v>44197.416666666701</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
-        <v>44197.458333333299</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
-        <v>44197.5</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
-        <v>44197.541666666701</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
-        <v>44197.583333333299</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -927,7 +926,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
-        <v>44197.625</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>22</v>
@@ -935,7 +934,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
-        <v>44197.666666666701</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>22</v>
@@ -943,7 +942,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
-        <v>44197.708333333299</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>22</v>
@@ -951,7 +950,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
-        <v>44197.75</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>22</v>
@@ -959,7 +958,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
-        <v>44197.791666666701</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -967,7 +966,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
-        <v>44197.833333333299</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -975,7 +974,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
-        <v>44197.875</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -983,7 +982,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
-        <v>44197.916666666701</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -991,7 +990,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
-        <v>44197.958333333299</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1003,22 +1002,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95034383-FE85-4F68-924D-0BEBCE2AD864}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555D891D-3F2A-4DCE-83B8-FA3AAFA767F2}">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="3"/>
+    <col min="1" max="1" width="25.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
@@ -1030,7 +1029,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>44197</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1041,7 +1040,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>44197.041666666664</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1052,7 +1051,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>44197.083333333299</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1063,7 +1062,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>44197.125</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1074,7 +1073,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
-        <v>44197.166666666701</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1085,183 +1084,183 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>44197.208333333299</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>44197.25</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>5.8000000000000003E-2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
-        <v>44197.291666666701</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>3.0000000000000001E-3</v>
+        <v>0.17</v>
       </c>
       <c r="C9">
-        <v>3.0000000000000001E-3</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>44197.333333333299</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>1.4E-2</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="C10">
-        <v>1.4E-2</v>
+        <v>0.32500000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>44197.375</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>3.0000000000000001E-3</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="C11">
-        <v>3.0000000000000001E-3</v>
+        <v>0.46899999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
-        <v>44197.416666666701</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>3.0000000000000001E-3</v>
+        <v>0.57199999999999995</v>
       </c>
       <c r="C12">
-        <v>3.0000000000000001E-3</v>
+        <v>0.57199999999999995</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
-        <v>44197.458333333299</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>0.63800000000000001</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.63800000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
-        <v>44197.5</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>1E-3</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="C14">
-        <v>1E-3</v>
+        <v>0.66500000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
-        <v>44197.541666666701</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>1.4999999999999999E-2</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="C15">
-        <v>1.4999999999999999E-2</v>
+        <v>0.63600000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
-        <v>44197.583333333299</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>0.60799999999999998</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>0.60799999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
-        <v>44197.625</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>0.54100000000000004</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>0.54100000000000004</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
-        <v>44197.666666666701</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>0.42599999999999999</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>0.42599999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
-        <v>44197.708333333299</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
-        <v>44197.75</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>0.14599999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
-        <v>44197.791666666701</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
-        <v>44197.833333333299</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
-        <v>44197.875</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -1272,7 +1271,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
-        <v>44197.916666666701</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1283,7 +1282,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
-        <v>44197.958333333299</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1295,4 +1294,383 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95034383-FE85-4F68-924D-0BEBCE2AD864}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F9">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1.4E-2</v>
+      </c>
+      <c r="C10">
+        <v>1.4E-2</v>
+      </c>
+      <c r="F10">
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F11">
+        <v>0.46899999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C12">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F12">
+        <v>0.57199999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0.63800000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1E-3</v>
+      </c>
+      <c r="C14">
+        <v>1E-3</v>
+      </c>
+      <c r="F14">
+        <v>0.66500000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C15">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.63600000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0.60799999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0.54100000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0.42599999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0.14599999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C0EF88-4887-4CA9-BA39-40AB3A7CB900}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added simple DSM - demand get be set up and down any time
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input.xlsx
+++ b/src/pv_optimizer_contracting/data_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723FA865-1564-4217-84EA-6E3E075477E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34203708-CFC1-4158-84DB-9D98D3E01F52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>PV</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Capacity limit grid</t>
+  </si>
+  <si>
+    <t>PV_ninja_21_7</t>
+  </si>
+  <si>
+    <t>PVGIS_EU</t>
   </si>
 </sst>
 </file>
@@ -641,7 +647,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -691,7 +697,7 @@
         <v>0.08</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -700,7 +706,7 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1006,7 +1012,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1087,10 +1093,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.01</v>
+        <v>0.1002</v>
       </c>
       <c r="C7">
-        <v>0.01</v>
+        <v>0.1002</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1098,10 +1104,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>5.8000000000000003E-2</v>
+        <v>0.26207999999999998</v>
       </c>
       <c r="C8">
-        <v>5.8000000000000003E-2</v>
+        <v>0.26207999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -1109,10 +1115,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.17</v>
+        <v>0.41768</v>
       </c>
       <c r="C9">
-        <v>0.17</v>
+        <v>0.41768</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1120,10 +1126,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.32500000000000001</v>
+        <v>0.55237000000000003</v>
       </c>
       <c r="C10">
-        <v>0.32500000000000001</v>
+        <v>0.55237000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1131,10 +1137,10 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.46899999999999997</v>
+        <v>0.48031999999999997</v>
       </c>
       <c r="C11">
-        <v>0.46899999999999997</v>
+        <v>0.48031999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -1142,10 +1148,10 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.57199999999999995</v>
+        <v>0.60196000000000005</v>
       </c>
       <c r="C12">
-        <v>0.57199999999999995</v>
+        <v>0.60196000000000005</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1153,10 +1159,10 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.63800000000000001</v>
+        <v>0.48791000000000001</v>
       </c>
       <c r="C13">
-        <v>0.63800000000000001</v>
+        <v>0.48791000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1164,10 +1170,10 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.66500000000000004</v>
+        <v>0.27662999999999999</v>
       </c>
       <c r="C14">
-        <v>0.66500000000000004</v>
+        <v>0.27662999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -1175,10 +1181,10 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.63600000000000001</v>
+        <v>0.19836000000000001</v>
       </c>
       <c r="C15">
-        <v>0.63600000000000001</v>
+        <v>0.19836000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1186,10 +1192,10 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.60799999999999998</v>
+        <v>0.25089</v>
       </c>
       <c r="C16">
-        <v>0.60799999999999998</v>
+        <v>0.25089</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1197,10 +1203,10 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.54100000000000004</v>
+        <v>0.21872999999999998</v>
       </c>
       <c r="C17">
-        <v>0.54100000000000004</v>
+        <v>0.21872999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1208,10 +1214,10 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.42599999999999999</v>
+        <v>7.6659999999999992E-2</v>
       </c>
       <c r="C18">
-        <v>0.42599999999999999</v>
+        <v>7.6659999999999992E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1219,10 +1225,10 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.28999999999999998</v>
+        <v>6.1600000000000005E-3</v>
       </c>
       <c r="C19">
-        <v>0.28999999999999998</v>
+        <v>6.1600000000000005E-3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1230,10 +1236,10 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.14599999999999999</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>0.14599999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -1241,10 +1247,10 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>4.4999999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>4.4999999999999998E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1252,10 +1258,10 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>7.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>7.0000000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -1298,10 +1304,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95034383-FE85-4F68-924D-0BEBCE2AD864}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1311,7 +1317,7 @@
     <col min="3" max="3" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1321,8 +1327,14 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1335,8 +1347,11 @@
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1349,8 +1364,11 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1363,8 +1381,11 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1377,8 +1398,11 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1391,8 +1415,11 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1405,8 +1432,11 @@
       <c r="F7">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7">
+        <v>0.1002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1419,8 +1449,11 @@
       <c r="F8">
         <v>5.8000000000000003E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8">
+        <v>0.26207999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1433,8 +1466,11 @@
       <c r="F9">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9">
+        <v>0.41768</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1447,8 +1483,11 @@
       <c r="F10">
         <v>0.32500000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10">
+        <v>0.55237000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1461,8 +1500,11 @@
       <c r="F11">
         <v>0.46899999999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11">
+        <v>0.48031999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1475,8 +1517,11 @@
       <c r="F12">
         <v>0.57199999999999995</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12">
+        <v>0.60196000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1489,8 +1534,11 @@
       <c r="F13">
         <v>0.63800000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13">
+        <v>0.48791000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1503,8 +1551,11 @@
       <c r="F14">
         <v>0.66500000000000004</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14">
+        <v>0.27662999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1517,8 +1568,11 @@
       <c r="F15">
         <v>0.63600000000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15">
+        <v>0.19836000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1531,8 +1585,11 @@
       <c r="F16">
         <v>0.60799999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16">
+        <v>0.25089</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1545,8 +1602,11 @@
       <c r="F17">
         <v>0.54100000000000004</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17">
+        <v>0.21872999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1559,8 +1619,11 @@
       <c r="F18">
         <v>0.42599999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18">
+        <v>7.6659999999999992E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1573,8 +1636,11 @@
       <c r="F19">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19">
+        <v>6.1600000000000005E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1587,8 +1653,11 @@
       <c r="F20">
         <v>0.14599999999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1601,8 +1670,11 @@
       <c r="F21">
         <v>4.4999999999999998E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1615,8 +1687,11 @@
       <c r="F22">
         <v>7.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1629,8 +1704,11 @@
       <c r="F23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1643,8 +1721,11 @@
       <c r="F24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1655,6 +1736,9 @@
         <v>0</v>
       </c>
       <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed all costs to simple dictionary
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input.xlsx
+++ b/src/pv_optimizer_contracting/data_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30891B0D-B4E7-467C-BB33-243093A8223B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755FFC03-D108-4ECC-92C0-B70B0A4C16C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -724,7 +724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33AEF11-6D95-4C68-8F05-ED28777DD177}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1017,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555D891D-3F2A-4DCE-83B8-FA3AAFA767F2}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C25"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>